<commit_message>
Creación de gráficas de las palabras más utilizadas en el idioma Español en la descripción corta y larga de los proyectos, además se crean la correspondientes gráficas del idioa Inglés
</commit_message>
<xml_diff>
--- a/text_analysis/data/short_description_words_cero_ESP.xlsx
+++ b/text_analysis/data/short_description_words_cero_ESP.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="1029">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="1027">
   <si>
     <t>niños</t>
   </si>
@@ -199,9 +199,6 @@
     <t>imagina</t>
   </si>
   <si>
-    <t>cada</t>
-  </si>
-  <si>
     <t>cultura</t>
   </si>
   <si>
@@ -260,9 +257,6 @@
   </si>
   <si>
     <t>mano</t>
-  </si>
-  <si>
-    <t>través</t>
   </si>
   <si>
     <t>hacemos</t>
@@ -3458,7 +3452,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1030"/>
+  <dimension ref="A1:C1028"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4470,7 +4464,7 @@
         <v>90</v>
       </c>
       <c r="C92">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -4481,7 +4475,7 @@
         <v>91</v>
       </c>
       <c r="C93">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -5812,7 +5806,7 @@
         <v>212</v>
       </c>
       <c r="C214">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="215" spans="1:3">
@@ -5823,7 +5817,7 @@
         <v>213</v>
       </c>
       <c r="C215">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="216" spans="1:3">
@@ -14766,28 +14760,6 @@
         <v>1026</v>
       </c>
       <c r="C1028">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1029" spans="1:3">
-      <c r="A1029" s="1">
-        <v>1027</v>
-      </c>
-      <c r="B1029" t="s">
-        <v>1027</v>
-      </c>
-      <c r="C1029">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1030" spans="1:3">
-      <c r="A1030" s="1">
-        <v>1028</v>
-      </c>
-      <c r="B1030" t="s">
-        <v>1028</v>
-      </c>
-      <c r="C1030">
         <v>1</v>
       </c>
     </row>

</xml_diff>